<commit_message>
associate file metadata in xls
</commit_message>
<xml_diff>
--- a/test_data/na_12879/na12879_accessioning.xlsx
+++ b/test_data/na_12879/na12879_accessioning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willronchetti/Documents/4dn/4dn-cloud-infra/test_data/na_12879/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6409D210-1266-A44A-AE76-40EF78F1C1A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2C97B-ABC8-6D4A-A5A1-730DC7B55CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="4100" windowWidth="33860" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Unique Analysis ID:</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>NA12877_sample</t>
+  </si>
+  <si>
+    <t>GAPFIHVO2FZQ.fastq.gz, GAPFIB4MJASV.fastq.gz</t>
+  </si>
+  <si>
+    <t>GAPFIK2ZO8UI.fastq.gz, GAPFIUCATWEO.fastq.gz</t>
+  </si>
+  <si>
+    <t>GAPFI1HVXJ5F.fastq.gz, GAPFIOFWFYZE.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -950,7 +959,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J2" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1026,6 +1035,9 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1055,6 +1067,9 @@
       <c r="I3" t="s">
         <v>12</v>
       </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1083,6 +1098,9 @@
       </c>
       <c r="I4" t="s">
         <v>12</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more documentation, repair xls, scripit
</commit_message>
<xml_diff>
--- a/test_data/na_12879/na12879_accessioning.xlsx
+++ b/test_data/na_12879/na12879_accessioning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willronchetti/Documents/4dn/4dn-cloud-infra/test_data/na_12879/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC2C97B-ABC8-6D4A-A5A1-730DC7B55CE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608AA333-86B8-B544-9AF5-92E6C96FF750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="4100" windowWidth="33860" windowHeight="15520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,13 +109,13 @@
     <t>NA12877_sample</t>
   </si>
   <si>
-    <t>GAPFIHVO2FZQ.fastq.gz, GAPFIB4MJASV.fastq.gz</t>
-  </si>
-  <si>
-    <t>GAPFIK2ZO8UI.fastq.gz, GAPFIUCATWEO.fastq.gz</t>
-  </si>
-  <si>
-    <t>GAPFI1HVXJ5F.fastq.gz, GAPFIOFWFYZE.fastq.gz</t>
+    <t>cgap:NA12879_sample_S1_R1, cgap:NA12879_sample_S1_R2</t>
+  </si>
+  <si>
+    <t>cgap:NA12878_sample_S1_R1, cgap:NA12878_sample_S1_R2</t>
+  </si>
+  <si>
+    <t>cgap:NA12877_sample_S1_R1, cgap:NA12877_sample_S1_R2</t>
   </si>
 </sst>
 </file>
@@ -959,7 +959,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>